<commit_message>
update for Admin flow and wireframe
</commit_message>
<xml_diff>
--- a/terms.xlsx
+++ b/terms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>English</t>
   </si>
@@ -178,7 +178,13 @@
     <t>系列</t>
   </si>
   <si>
-    <t>a section of a course with a specific learning purpose</t>
+    <t>a particular section of a course with a specific learning purpose. A course is composed of a series of sequences</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>等级</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -745,7 +751,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -754,6 +760,14 @@
       </c>
       <c r="C19" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>